<commit_message>
storing maintenance properties to config
</commit_message>
<xml_diff>
--- a/uploads/CHG040422.xlsx
+++ b/uploads/CHG040422.xlsx
@@ -1,108 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRIMANDARBHA\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AFAD33-19B8-45A8-BAC4-F9F46B816D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D582576B-7699-4AD6-8BB2-43C0477EDFB4}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>server1</t>
-  </si>
-  <si>
-    <t>admin@example.com</t>
-  </si>
-  <si>
-    <t>/u01</t>
-  </si>
-  <si>
-    <t>EMAX100</t>
-  </si>
-  <si>
-    <t>Dell Clairon</t>
-  </si>
-  <si>
-    <t>CHG040422</t>
-  </si>
-  <si>
-    <t>servers</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>array</t>
-  </si>
-  <si>
-    <t>storage</t>
-  </si>
-  <si>
-    <t>enddate</t>
-  </si>
-  <si>
-    <t>SNOW change</t>
-  </si>
-  <si>
-    <t>maintenance_name</t>
-  </si>
-  <si>
-    <t>Dell Migration</t>
-  </si>
-  <si>
-    <t>server2</t>
-  </si>
-  <si>
-    <t>/u02</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -121,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -436,98 +420,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FCB5C7-4F1B-4D66-9B92-3033CFCCF2AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="59.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col width="59.21875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="19" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.33203125" bestFit="1" customWidth="1" min="5" max="6"/>
+    <col width="10.5546875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="17.33203125" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>servers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>path</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>storage</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>enddate</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>SNOW change</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>maintenance_name</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>server1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>admin@example.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>/u01</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EMAX100</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Dell Clairon</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>45504</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CHG040422</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Dell Migration</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>admin@example.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>/u02</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>EMAX100</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Dell Clairon</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>45504</v>
       </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CHG040422</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Dell Migration</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new schedules function
</commit_message>
<xml_diff>
--- a/uploads/CHG040422.xlsx
+++ b/uploads/CHG040422.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -508,9 +508,7 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F2" s="1" t="n">
-        <v>45504</v>
-      </c>
+      <c r="F2" s="1" t="n"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>CHG040422</t>
@@ -548,9 +546,7 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>45504</v>
-      </c>
+      <c r="F3" s="1" t="n"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>CHG040422</t>

</xml_diff>

<commit_message>
selectall and maint listing
</commit_message>
<xml_diff>
--- a/uploads/CHG040422.xlsx
+++ b/uploads/CHG040422.xlsx
@@ -519,7 +519,11 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F2" s="1" t="n"/>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>2024-08-03</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>CHG040422</t>

</xml_diff>

<commit_message>
data saving for individual level
</commit_message>
<xml_diff>
--- a/uploads/CHG040422.xlsx
+++ b/uploads/CHG040422.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>2024-08-03</t>
+          <t>2024-08-10</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -789,7 +789,11 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F9" s="1" t="n"/>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>2024-08-10</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>CHG040422</t>

</xml_diff>

<commit_message>
partially fixed adding data back to excel
</commit_message>
<xml_diff>
--- a/uploads/CHG040422.xlsx
+++ b/uploads/CHG040422.xlsx
@@ -606,7 +606,11 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F4" s="1" t="n"/>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>2024-08-04</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>CHG040422</t>
@@ -615,6 +619,16 @@
       <c r="H4" t="inlineStr">
         <is>
           <t>Dell Migration</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -682,7 +696,11 @@
           <t>Dell Clairon</t>
         </is>
       </c>
-      <c r="F6" s="1" t="n"/>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>2024-08-04</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>CHG040422</t>
@@ -691,6 +709,16 @@
       <c r="H6" t="inlineStr">
         <is>
           <t>Dell Migration</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>